<commit_message>
VERSION 1.0 - MAQUINA SIN IA
</commit_message>
<xml_diff>
--- a/Cajas negras/Combate/Entrenador.xlsx
+++ b/Cajas negras/Combate/Entrenador.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1º Ciclo Superior DAM 2018-2019\Programación\3º Trimestre\Proyecto Pokemon\Cajas negras\Combate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esther\eclipse-workspace\Pokemon\Cajas negras\Combate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8760"/>
   </bookViews>
   <sheets>
-    <sheet name="Constructor" sheetId="1" r:id="rId1"/>
-    <sheet name="areAllPokemonsAlive()" sheetId="3" r:id="rId2"/>
-    <sheet name="luchar()" sheetId="6" r:id="rId3"/>
-    <sheet name="asignarPokemons()" sheetId="7" r:id="rId4"/>
-    <sheet name="cambiar()" sheetId="9" r:id="rId5"/>
-    <sheet name="seleccionarOpcion()" sheetId="8" r:id="rId6"/>
+    <sheet name="areAllPokemonsAlive()" sheetId="3" r:id="rId1"/>
+    <sheet name="luchar()" sheetId="6" r:id="rId2"/>
+    <sheet name="asignarPokemons()" sheetId="7" r:id="rId3"/>
+    <sheet name="cambiar()" sheetId="9" r:id="rId4"/>
+    <sheet name="seleccionarOpcion()" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
   <si>
     <t>Clases de equivalencia válidas</t>
   </si>
@@ -56,15 +55,6 @@
   </si>
   <si>
     <t>atacar(int ataque, Pokemon oponente)</t>
-  </si>
-  <si>
-    <t>Entrenador(String nombre)</t>
-  </si>
-  <si>
-    <t>nombre == null</t>
-  </si>
-  <si>
-    <t>nombre = ""</t>
   </si>
   <si>
     <t>Al menos un pokemon con vida</t>
@@ -190,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -256,19 +246,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -309,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -323,43 +300,40 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -642,105 +616,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="5" max="5" width="23.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="42.6" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" ht="55.2" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.8">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" ht="24.6" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="21.6" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -751,49 +629,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="42.6" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="55.2" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" ht="43.2">
       <c r="A4" s="4" t="s">
@@ -802,10 +680,10 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -817,10 +695,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -847,7 +725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -862,14 +740,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="42.6" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="A1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="41.4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.2" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="42.6" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="55.2">
       <c r="A2" s="1" t="s">
@@ -878,37 +830,37 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.2" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.8">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+    <row r="3" spans="1:6" ht="57.6">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" ht="43.2">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -927,23 +879,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6" ht="42.6" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="55.2">
       <c r="A2" s="1" t="s">
@@ -952,40 +904,54 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.6">
+    <row r="3" spans="1:6" ht="43.2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="43.2">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" ht="28.8">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="43.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1004,108 +970,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="42.6" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="55.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="43.2">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.8">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="43.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6" ht="42.6" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="A1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="55.2">
       <c r="A2" s="1" t="s">
@@ -1114,47 +992,47 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="17">
+      <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="D4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="28.8">
-      <c r="A5" s="14"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1162,8 +1040,8 @@
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>30</v>
+      <c r="E5" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="F5" s="3"/>
     </row>

</xml_diff>